<commit_message>
commit by jar :: 단체등록엑셀
</commit_message>
<xml_diff>
--- a/F-EMS/src/main/webapp/resources/files/교수등록.xlsx
+++ b/F-EMS/src/main/webapp/resources/files/교수등록.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="28035" windowHeight="12555"/>
@@ -11,70 +11,52 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>교수번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비밀번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>학과코드</t>
   </si>
   <si>
     <t>이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>영문이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>주민번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>핸드폰번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>집 전화번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우편번호</t>
+  </si>
+  <si>
+    <t>주소</t>
+  </si>
+  <si>
+    <t>이메일</t>
+  </si>
+  <si>
+    <t>상세 주소</t>
+  </si>
+  <si>
+    <t>핸드폰 번호</t>
   </si>
   <si>
     <t>교수 전화번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>우편번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상세주소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이메일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>학과</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,7 +212,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -265,7 +246,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -441,35 +421,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -478,22 +462,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -504,12 +482,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -517,12 +495,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>